<commit_message>
Implemented a New Randomizer Function
</commit_message>
<xml_diff>
--- a/backend/resources/excel/Participants.xlsx
+++ b/backend/resources/excel/Participants.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17880" windowHeight="12180"/>
+    <workbookView windowWidth="14400" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
   <si>
     <t>EMPID</t>
   </si>
@@ -48,13 +48,13 @@
     <t>SMITH, JOHN D.</t>
   </si>
   <si>
-    <t>Zephyr Innovations</t>
+    <t>VIVA ARTISTS AGENCY, INC.</t>
   </si>
   <si>
     <t>JOHNSON, WILLIAM M.</t>
   </si>
   <si>
-    <t>Ember Dynamics</t>
+    <t>VICOR MUSIC CORP.</t>
   </si>
   <si>
     <t>BROWN, JAMES A.</t>
@@ -63,19 +63,19 @@
     <t>JONES, ROBERT B.</t>
   </si>
   <si>
-    <t>Astral Commerce</t>
+    <t>VIVA MUSIC PUBLISHING, INC.</t>
   </si>
   <si>
     <t>MILLER, DAVID C.</t>
   </si>
   <si>
-    <t>Nimbus Consulting</t>
+    <t>OC PRODUCTIONS AND ENTERTAINMENT, INC.</t>
   </si>
   <si>
     <t>DAVIS, JOSEPH E.</t>
   </si>
   <si>
-    <t>Verdant Horizons Enterprises</t>
+    <t>ULTIMATE ENTERTAINMENT, INC.</t>
   </si>
   <si>
     <t>GARCIA, RICHARD F.</t>
@@ -87,7 +87,7 @@
     <t>WILSON, THOMAS H.</t>
   </si>
   <si>
-    <t>Quantum Nexus Corporation</t>
+    <t>VIVA LIVE, INC.</t>
   </si>
   <si>
     <t>MARTINEZ, DANIEL I.</t>
@@ -108,7 +108,7 @@
     <t>CLARK, ANTHONY N.</t>
   </si>
   <si>
-    <t>Terra Firma Industries</t>
+    <t>VIVA BOOKS PUBLISHING, INC.</t>
   </si>
   <si>
     <t>LEWIS, MARK O.</t>
@@ -126,7 +126,7 @@
     <t>LEE, WILLIAM S.</t>
   </si>
   <si>
-    <t>Obsidian Digital Solutions</t>
+    <t>VIVA LIFESTYLE and LEISURE, INC.</t>
   </si>
   <si>
     <t>WALKER, RICHARD T.</t>
@@ -153,7 +153,7 @@
     <t>PRICE, MARK A.</t>
   </si>
   <si>
-    <t>Cerulean Energy Group</t>
+    <t>VIVA RECORDS CORP.</t>
   </si>
   <si>
     <t>BAKER, STEVEN B.</t>
@@ -186,10 +186,13 @@
     <t>PHILLIPS, DANIEL K.</t>
   </si>
   <si>
+    <t>VIVA COMMUNICATIONS, INC.</t>
+  </si>
+  <si>
     <t>CAMPBELL, PATRICK L.</t>
   </si>
   <si>
-    <t>NovaTech Systems</t>
+    <t>EPIK STUDIOS, INC.</t>
   </si>
   <si>
     <t>PARKER, JAMES M.</t>
@@ -202,6 +205,9 @@
   </si>
   <si>
     <t>COLLINS, RICHARD P.</t>
+  </si>
+  <si>
+    <t>VIVA INTERNATIONAL FOOD &amp; RESTAURANTS, INC.</t>
   </si>
   <si>
     <t>STEWART, CHARLES Q.</t>
@@ -1377,8 +1383,8 @@
   <sheetPr/>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="N55" sqref="N55"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1928,10 +1934,10 @@
         <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D39">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1939,10 +1945,10 @@
         <v>139</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D40">
         <v>5</v>
@@ -1953,10 +1959,10 @@
         <v>140</v>
       </c>
       <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" t="s">
         <v>53</v>
-      </c>
-      <c r="C41" t="s">
-        <v>52</v>
       </c>
       <c r="D41">
         <v>5</v>
@@ -1967,13 +1973,13 @@
         <v>141</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D42">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1981,10 +1987,10 @@
         <v>142</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -1995,13 +2001,13 @@
         <v>143</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D44">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2009,7 +2015,7 @@
         <v>144</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
         <v>18</v>
@@ -2023,13 +2029,13 @@
         <v>145</v>
       </c>
       <c r="B46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" t="s">
         <v>58</v>
       </c>
-      <c r="C46" t="s">
-        <v>18</v>
-      </c>
       <c r="D46">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2037,7 +2043,7 @@
         <v>146</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C47" t="s">
         <v>25</v>
@@ -2051,10 +2057,10 @@
         <v>147</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D48">
         <v>5</v>
@@ -2065,7 +2071,7 @@
         <v>148</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C49" t="s">
         <v>25</v>
@@ -2079,13 +2085,13 @@
         <v>149</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2093,17 +2099,17 @@
         <v>150</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C51" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D51">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:D51" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2117,7 +2123,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>